<commit_message>
calibrate pot to degrees
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -856,194 +856,74 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>

</xml_diff>